<commit_message>
coverage of remainig cases
</commit_message>
<xml_diff>
--- a/VonageConversationsApi Cases.xlsx
+++ b/VonageConversationsApi Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="488">
   <si>
     <t>Module</t>
   </si>
@@ -1235,6 +1235,15 @@
     <t>verify user is not able to add same member again  and response is as expected as per the matrix table</t>
   </si>
   <si>
+    <t>verify user is able to create member with all different channels</t>
+  </si>
+  <si>
+    <t>verify user is able to create a member with mandatory fields alone</t>
+  </si>
+  <si>
+    <t>open for clarification, mandtory fields are not as per the document</t>
+  </si>
+  <si>
     <t>verify user is not able to fetch a member with invalid member id and get 404 with response body as expected as per the test case matrix</t>
   </si>
   <si>
@@ -1295,13 +1304,13 @@
     <t>verify user is able to add same event again  and response is as expected as per the matrix table</t>
   </si>
   <si>
+    <t>verify user is not able to create event before the members become to joined state</t>
+  </si>
+  <si>
     <t>verify user is not able to fetch a event with invalid event/ conversation id and get 404 with response body as expected as per the test case matrix</t>
   </si>
   <si>
-    <t>verify user is not able to get deleted event</t>
-  </si>
-  <si>
-    <t>verify user is able to get latest values after updating the event</t>
+    <t>verify user is able to get deleted event</t>
   </si>
   <si>
     <t>verify user is not able to delete an event with invalid conversation/event id and gets 404 with response body as expected as per the test case matrix</t>
@@ -1310,6 +1319,9 @@
     <t>verify user is not able to delete an alaredy deleted event</t>
   </si>
   <si>
+    <t>open forclarification</t>
+  </si>
+  <si>
     <t>verify when the application has data the api lists all the legs with expected fields as listed in the test case matrix</t>
   </si>
   <si>
@@ -1350,6 +1362,15 @@
   </si>
   <si>
     <t>verify the endpoints fail with 500 with respective error messag incase of unhandled expections</t>
+  </si>
+  <si>
+    <t>Funcational</t>
+  </si>
+  <si>
+    <t>verify Events and members are deleted when a conversation is deleted</t>
+  </si>
+  <si>
+    <t>verify members are deleted when a user is deleted</t>
   </si>
   <si>
     <t>Response Fields</t>
@@ -14137,7 +14158,7 @@
     <col customWidth="1" min="2" max="2" width="18.5"/>
     <col customWidth="1" min="3" max="3" width="11.13"/>
     <col customWidth="1" min="4" max="4" width="44.63"/>
-    <col customWidth="1" min="5" max="5" width="117.0"/>
+    <col customWidth="1" min="5" max="5" width="122.0"/>
     <col customWidth="1" min="6" max="6" width="15.75"/>
   </cols>
   <sheetData>
@@ -14934,6 +14955,9 @@
       <c r="E74" s="7" t="s">
         <v>167</v>
       </c>
+      <c r="F74" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G74" s="7" t="s">
         <v>169</v>
       </c>
@@ -14956,6 +14980,9 @@
       <c r="E76" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="F76" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G76" s="7" t="s">
         <v>169</v>
       </c>
@@ -14967,6 +14994,9 @@
       <c r="E77" s="7" t="s">
         <v>230</v>
       </c>
+      <c r="F77" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="78">
       <c r="B78" s="7"/>
@@ -14975,6 +15005,9 @@
       <c r="E78" s="7" t="s">
         <v>231</v>
       </c>
+      <c r="F78" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G78" s="7" t="s">
         <v>232</v>
       </c>
@@ -14986,6 +15019,9 @@
       <c r="E79" s="7" t="s">
         <v>176</v>
       </c>
+      <c r="F79" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="80">
       <c r="B80" s="7"/>
@@ -14994,6 +15030,9 @@
       <c r="E80" s="7" t="s">
         <v>233</v>
       </c>
+      <c r="F80" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G80" s="7"/>
     </row>
     <row r="81">
@@ -15008,6 +15047,9 @@
       </c>
       <c r="E81" s="7" t="s">
         <v>167</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>169</v>
@@ -15031,6 +15073,9 @@
       <c r="E83" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="F83" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G83" s="7" t="s">
         <v>169</v>
       </c>
@@ -15042,6 +15087,9 @@
       <c r="E84" s="7" t="s">
         <v>234</v>
       </c>
+      <c r="F84" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" s="7"/>
@@ -15050,6 +15098,9 @@
       <c r="E85" s="7" t="s">
         <v>235</v>
       </c>
+      <c r="F85" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="86">
       <c r="B86" s="7"/>
@@ -15058,6 +15109,9 @@
       <c r="E86" s="7" t="s">
         <v>236</v>
       </c>
+      <c r="F86" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G86" s="7" t="s">
         <v>191</v>
       </c>
@@ -15069,6 +15123,9 @@
       <c r="E87" s="7" t="s">
         <v>237</v>
       </c>
+      <c r="F87" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G87" s="7"/>
     </row>
     <row r="88">
@@ -15078,6 +15135,9 @@
       <c r="E88" s="7" t="s">
         <v>238</v>
       </c>
+      <c r="F88" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G88" s="7" t="s">
         <v>239</v>
       </c>
@@ -15094,6 +15154,9 @@
       </c>
       <c r="E89" s="7" t="s">
         <v>167</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>207</v>
@@ -15117,6 +15180,9 @@
       <c r="E91" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="F91" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G91" s="7" t="s">
         <v>207</v>
       </c>
@@ -15128,6 +15194,9 @@
       <c r="E92" s="7" t="s">
         <v>176</v>
       </c>
+      <c r="F92" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="93">
       <c r="B93" s="7"/>
@@ -15136,6 +15205,9 @@
       <c r="E93" s="7" t="s">
         <v>240</v>
       </c>
+      <c r="F93" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="7"/>
@@ -15144,6 +15216,9 @@
       <c r="E94" s="7" t="s">
         <v>241</v>
       </c>
+      <c r="F94" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="95">
       <c r="B95" s="7"/>
@@ -15152,6 +15227,9 @@
       <c r="E95" s="7" t="s">
         <v>242</v>
       </c>
+      <c r="F95" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G95" s="7" t="s">
         <v>243</v>
       </c>
@@ -15168,6 +15246,9 @@
       </c>
       <c r="E96" s="7" t="s">
         <v>167</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>194</v>
@@ -15191,6 +15272,9 @@
       <c r="E98" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="F98" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G98" s="7" t="s">
         <v>194</v>
       </c>
@@ -15202,6 +15286,9 @@
       <c r="E99" s="7" t="s">
         <v>244</v>
       </c>
+      <c r="F99" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" s="7"/>
@@ -15210,6 +15297,9 @@
       <c r="E100" s="7" t="s">
         <v>245</v>
       </c>
+      <c r="F100" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="101">
       <c r="B101" s="7"/>
@@ -15226,6 +15316,9 @@
       <c r="E102" s="7" t="s">
         <v>247</v>
       </c>
+      <c r="F102" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" s="7"/>
@@ -15234,6 +15327,9 @@
       <c r="E103" s="7" t="s">
         <v>199</v>
       </c>
+      <c r="F103" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="104">
       <c r="B104" s="7"/>
@@ -15242,6 +15338,9 @@
       <c r="E104" s="7" t="s">
         <v>202</v>
       </c>
+      <c r="F104" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G104" s="7"/>
     </row>
     <row r="105">
@@ -15260,6 +15359,9 @@
       <c r="E106" s="7" t="s">
         <v>248</v>
       </c>
+      <c r="F106" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G106" s="7"/>
     </row>
     <row r="107">
@@ -15269,6 +15371,9 @@
       <c r="E107" s="7" t="s">
         <v>249</v>
       </c>
+      <c r="F107" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G107" s="7"/>
     </row>
     <row r="108">
@@ -15278,6 +15383,9 @@
       <c r="E108" s="7" t="s">
         <v>250</v>
       </c>
+      <c r="F108" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G108" s="7"/>
     </row>
     <row r="109">
@@ -15292,6 +15400,9 @@
       </c>
       <c r="E109" s="7" t="s">
         <v>167</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G109" s="7" t="s">
         <v>207</v>
@@ -15315,6 +15426,9 @@
       <c r="E111" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="F111" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G111" s="7" t="s">
         <v>207</v>
       </c>
@@ -15326,6 +15440,9 @@
       <c r="E112" s="7" t="s">
         <v>212</v>
       </c>
+      <c r="F112" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="113">
       <c r="B113" s="7"/>
@@ -15334,6 +15451,9 @@
       <c r="E113" s="7" t="s">
         <v>251</v>
       </c>
+      <c r="F113" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="114">
       <c r="B114" s="7"/>
@@ -15341,6 +15461,9 @@
       <c r="D114" s="7"/>
       <c r="E114" s="7" t="s">
         <v>252</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="115">
@@ -15403,6 +15526,9 @@
       <c r="E119" s="7" t="s">
         <v>257</v>
       </c>
+      <c r="F119" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="120">
       <c r="B120" s="7"/>
@@ -15411,6 +15537,9 @@
       <c r="E120" s="7" t="s">
         <v>258</v>
       </c>
+      <c r="F120" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="121">
       <c r="B121" s="7"/>
@@ -15419,6 +15548,9 @@
       <c r="E121" s="7" t="s">
         <v>259</v>
       </c>
+      <c r="F121" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="122">
       <c r="B122" s="7"/>
@@ -15427,6 +15559,9 @@
       <c r="E122" s="7" t="s">
         <v>260</v>
       </c>
+      <c r="F122" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="123">
       <c r="B123" s="7"/>
@@ -15435,6 +15570,9 @@
       <c r="E123" s="7" t="s">
         <v>261</v>
       </c>
+      <c r="F123" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="124">
       <c r="B124" s="7"/>
@@ -15443,6 +15581,9 @@
       <c r="E124" s="7" t="s">
         <v>262</v>
       </c>
+      <c r="F124" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="G124" s="7" t="s">
         <v>239</v>
       </c>
@@ -15459,6 +15600,9 @@
       </c>
       <c r="E125" s="7" t="s">
         <v>263</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G125" s="7" t="s">
         <v>239</v>
@@ -15471,6 +15615,9 @@
       <c r="E126" s="7" t="s">
         <v>264</v>
       </c>
+      <c r="F126" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="127">
       <c r="B127" s="7"/>
@@ -15479,6 +15626,9 @@
       <c r="E127" s="7" t="s">
         <v>265</v>
       </c>
+      <c r="F127" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="128">
       <c r="B128" s="7"/>
@@ -15487,6 +15637,9 @@
       <c r="E128" s="7" t="s">
         <v>266</v>
       </c>
+      <c r="F128" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="129">
       <c r="B129" s="7"/>
@@ -15495,6 +15648,9 @@
       <c r="E129" s="7" t="s">
         <v>267</v>
       </c>
+      <c r="F129" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="130">
       <c r="B130" s="7"/>
@@ -15503,44 +15659,45 @@
       <c r="E130" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="G130" s="7" t="s">
-        <v>239</v>
+      <c r="F130" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="131">
-      <c r="B131" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C131" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="B131" s="7"/>
+      <c r="C131" s="22"/>
+      <c r="D131" s="7"/>
       <c r="E131" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G131" s="7" t="s">
-        <v>207</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="G131" s="7"/>
     </row>
     <row r="132">
       <c r="B132" s="7"/>
       <c r="C132" s="22"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7" t="s">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>207</v>
+        <v>271</v>
       </c>
     </row>
     <row r="133">
-      <c r="B133" s="7"/>
-      <c r="C133" s="22"/>
-      <c r="D133" s="7"/>
+      <c r="B133" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="E133" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G133" s="7" t="s">
         <v>207</v>
@@ -15551,7 +15708,10 @@
       <c r="C134" s="22"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
+      </c>
+      <c r="G134" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="135">
@@ -15559,7 +15719,13 @@
       <c r="C135" s="22"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7" t="s">
-        <v>269</v>
+        <v>172</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="136">
@@ -15567,7 +15733,10 @@
       <c r="C136" s="22"/>
       <c r="D136" s="7"/>
       <c r="E136" s="7" t="s">
-        <v>270</v>
+        <v>176</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="137">
@@ -15575,27 +15744,21 @@
       <c r="C137" s="22"/>
       <c r="D137" s="7"/>
       <c r="E137" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="G137" s="7" t="s">
-        <v>243</v>
+        <v>272</v>
+      </c>
+      <c r="F137" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="138">
-      <c r="B138" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C138" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="B138" s="7"/>
+      <c r="C138" s="22"/>
+      <c r="D138" s="7"/>
       <c r="E138" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>194</v>
+        <v>273</v>
+      </c>
+      <c r="F138" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="139">
@@ -15603,18 +15766,30 @@
       <c r="C139" s="22"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7" t="s">
-        <v>170</v>
+        <v>274</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
     </row>
     <row r="140">
-      <c r="B140" s="7"/>
-      <c r="C140" s="22"/>
-      <c r="D140" s="7"/>
+      <c r="B140" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="E140" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="F140" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G140" s="7" t="s">
         <v>194</v>
@@ -15625,7 +15800,10 @@
       <c r="C141" s="22"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7" t="s">
-        <v>272</v>
+        <v>170</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="142">
@@ -15633,7 +15811,13 @@
       <c r="C142" s="22"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7" t="s">
-        <v>273</v>
+        <v>172</v>
+      </c>
+      <c r="F142" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G142" s="7" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="143">
@@ -15641,7 +15825,10 @@
       <c r="C143" s="22"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="F143" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="144">
@@ -15649,7 +15836,10 @@
       <c r="C144" s="22"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="F144" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="145">
@@ -15657,7 +15847,10 @@
       <c r="C145" s="22"/>
       <c r="D145" s="7"/>
       <c r="E145" s="7" t="s">
-        <v>199</v>
+        <v>277</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="146">
@@ -15665,25 +15858,29 @@
       <c r="C146" s="22"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G146" s="7"/>
+        <v>278</v>
+      </c>
+      <c r="F146" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="147">
       <c r="B147" s="7"/>
       <c r="C147" s="22"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="G147" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="F147" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="148">
       <c r="B148" s="7"/>
       <c r="C148" s="22"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="G148" s="7"/>
     </row>
@@ -15692,7 +15889,10 @@
       <c r="C149" s="22"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7" t="s">
-        <v>249</v>
+        <v>203</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G149" s="7"/>
     </row>
@@ -15701,45 +15901,51 @@
       <c r="C150" s="22"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7" t="s">
-        <v>277</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F150" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G150" s="7"/>
     </row>
     <row r="151">
-      <c r="B151" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C151" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D151" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="B151" s="7"/>
+      <c r="C151" s="22"/>
+      <c r="D151" s="7"/>
       <c r="E151" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G151" s="7" t="s">
-        <v>207</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G151" s="7"/>
     </row>
     <row r="152">
-      <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="22"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G152" s="7" t="s">
-        <v>207</v>
+        <v>280</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="22"/>
-      <c r="D153" s="7"/>
+      <c r="B153" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="E153" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="F153" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G153" s="7" t="s">
         <v>207</v>
@@ -15751,7 +15957,10 @@
       <c r="C154" s="22"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7" t="s">
-        <v>212</v>
+        <v>170</v>
+      </c>
+      <c r="G154" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="155">
@@ -15760,7 +15969,13 @@
       <c r="C155" s="22"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7" t="s">
-        <v>278</v>
+        <v>172</v>
+      </c>
+      <c r="F155" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="156">
@@ -15769,40 +15984,54 @@
       <c r="C156" s="22"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7" t="s">
-        <v>279</v>
+        <v>212</v>
+      </c>
+      <c r="F156" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C157" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D157" s="7" t="s">
-        <v>134</v>
-      </c>
+      <c r="A157" s="7"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="22"/>
+      <c r="D157" s="7"/>
       <c r="E157" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="F157" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="158">
+      <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="22"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="F158" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="159">
-      <c r="B159" s="7"/>
-      <c r="C159" s="22"/>
-      <c r="D159" s="7"/>
+      <c r="A159" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C159" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="E159" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="160">
@@ -15810,7 +16039,10 @@
       <c r="C160" s="22"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="161">
@@ -15818,7 +16050,10 @@
       <c r="C161" s="22"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
+      </c>
+      <c r="F161" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="162">
@@ -15826,27 +16061,21 @@
       <c r="C162" s="22"/>
       <c r="D162" s="7"/>
       <c r="E162" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="G162" s="7" t="s">
-        <v>239</v>
+        <v>286</v>
+      </c>
+      <c r="F162" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="163">
-      <c r="B163" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C163" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D163" s="7" t="s">
-        <v>134</v>
-      </c>
+      <c r="B163" s="7"/>
+      <c r="C163" s="22"/>
+      <c r="D163" s="7"/>
       <c r="E163" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="G163" s="7" t="s">
-        <v>239</v>
+        <v>287</v>
+      </c>
+      <c r="F163" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="164">
@@ -15854,15 +16083,33 @@
       <c r="C164" s="22"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7" t="s">
-        <v>285</v>
+        <v>262</v>
+      </c>
+      <c r="F164" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G164" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="165">
-      <c r="B165" s="7"/>
-      <c r="C165" s="22"/>
-      <c r="D165" s="7"/>
+      <c r="B165" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="E165" s="7" t="s">
-        <v>286</v>
+        <v>263</v>
+      </c>
+      <c r="F165" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G165" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="166">
@@ -15870,7 +16117,10 @@
       <c r="C166" s="22"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
+      </c>
+      <c r="F166" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="167">
@@ -15878,7 +16128,10 @@
       <c r="C167" s="22"/>
       <c r="D167" s="7"/>
       <c r="E167" s="7" t="s">
-        <v>267</v>
+        <v>289</v>
+      </c>
+      <c r="F167" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="168">
@@ -15886,27 +16139,21 @@
       <c r="C168" s="22"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="G168" s="7" t="s">
-        <v>239</v>
+        <v>290</v>
+      </c>
+      <c r="F168" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="169">
-      <c r="B169" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C169" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D169" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="B169" s="7"/>
+      <c r="C169" s="22"/>
+      <c r="D169" s="7"/>
       <c r="E169" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G169" s="7" t="s">
-        <v>207</v>
+        <v>267</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="170">
@@ -15914,10 +16161,13 @@
       <c r="C170" s="22"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7" t="s">
-        <v>170</v>
+        <v>291</v>
+      </c>
+      <c r="F170" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
     </row>
     <row r="171">
@@ -15925,18 +16175,28 @@
       <c r="C171" s="22"/>
       <c r="D171" s="7"/>
       <c r="E171" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G171" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G171" s="7"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C172" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D172" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E172" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F172" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G172" s="7" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="B172" s="7"/>
-      <c r="C172" s="22"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="173">
@@ -15944,7 +16204,10 @@
       <c r="C173" s="22"/>
       <c r="D173" s="7"/>
       <c r="E173" s="7" t="s">
-        <v>289</v>
+        <v>170</v>
+      </c>
+      <c r="G173" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="174">
@@ -15952,7 +16215,13 @@
       <c r="C174" s="22"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7" t="s">
-        <v>290</v>
+        <v>172</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G174" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="175">
@@ -15960,48 +16229,49 @@
       <c r="C175" s="22"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="G175" s="7" t="s">
-        <v>243</v>
+        <v>176</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="176">
-      <c r="B176" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C176" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D176" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="B176" s="7"/>
+      <c r="C176" s="22"/>
+      <c r="D176" s="7"/>
       <c r="E176" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G176" s="7" t="s">
-        <v>207</v>
+        <v>293</v>
+      </c>
+      <c r="F176" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="22"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G177" s="7" t="s">
-        <v>207</v>
+        <v>294</v>
+      </c>
+      <c r="F177" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="22"/>
-      <c r="D178" s="7"/>
+      <c r="B178" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C178" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="E178" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="F178" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G178" s="7" t="s">
         <v>207</v>
@@ -16013,7 +16283,10 @@
       <c r="C179" s="22"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7" t="s">
-        <v>212</v>
+        <v>170</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="180">
@@ -16022,7 +16295,13 @@
       <c r="C180" s="22"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7" t="s">
-        <v>292</v>
+        <v>172</v>
+      </c>
+      <c r="F180" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G180" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="181">
@@ -16031,49 +16310,51 @@
       <c r="C181" s="22"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7" t="s">
-        <v>293</v>
+        <v>212</v>
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B182" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C182" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="22"/>
+      <c r="D182" s="7"/>
       <c r="E182" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G182" s="7" t="s">
-        <v>169</v>
+        <v>295</v>
+      </c>
+      <c r="F182" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="183">
+      <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="22"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F183" s="7" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="G183" s="7" t="s">
-        <v>169</v>
+        <v>297</v>
       </c>
     </row>
     <row r="184">
-      <c r="B184" s="7"/>
-      <c r="C184" s="22"/>
-      <c r="D184" s="7"/>
+      <c r="A184" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C184" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D184" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="E184" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="F184" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G184" s="7" t="s">
         <v>169</v>
@@ -16084,7 +16365,13 @@
       <c r="C185" s="22"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="F185" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G185" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="186">
@@ -16092,7 +16379,13 @@
       <c r="C186" s="22"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7" t="s">
-        <v>294</v>
+        <v>172</v>
+      </c>
+      <c r="F186" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G186" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="187">
@@ -16100,7 +16393,10 @@
       <c r="C187" s="22"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
+      </c>
+      <c r="F187" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="188">
@@ -16108,7 +16404,7 @@
       <c r="C188" s="22"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7" t="s">
-        <v>177</v>
+        <v>298</v>
       </c>
     </row>
     <row r="189">
@@ -16116,7 +16412,7 @@
       <c r="C189" s="22"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="190">
@@ -16124,7 +16420,7 @@
       <c r="C190" s="22"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="191">
@@ -16132,44 +16428,44 @@
       <c r="C191" s="22"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="G191" s="7"/>
+        <v>183</v>
+      </c>
     </row>
     <row r="192">
+      <c r="B192" s="7"/>
+      <c r="C192" s="22"/>
+      <c r="D192" s="7"/>
       <c r="E192" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="G192" s="7"/>
+        <v>184</v>
+      </c>
     </row>
     <row r="193">
-      <c r="B193" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C193" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D193" s="7" t="s">
-        <v>152</v>
-      </c>
+      <c r="B193" s="7"/>
+      <c r="C193" s="22"/>
+      <c r="D193" s="7"/>
       <c r="E193" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G193" s="7" t="s">
-        <v>207</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="G193" s="7"/>
     </row>
     <row r="194">
       <c r="E194" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G194" s="7" t="s">
-        <v>207</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="G194" s="7"/>
     </row>
     <row r="195">
+      <c r="B195" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C195" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="E195" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G195" s="7" t="s">
         <v>207</v>
@@ -16177,54 +16473,95 @@
     </row>
     <row r="196">
       <c r="E196" s="7" t="s">
-        <v>212</v>
+        <v>170</v>
+      </c>
+      <c r="G196" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="197">
       <c r="E197" s="7" t="s">
-        <v>297</v>
+        <v>172</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="198">
       <c r="E198" s="7" t="s">
-        <v>298</v>
+        <v>212</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C199" s="7" t="s">
+      <c r="E199" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="D199" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E199" s="7" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="200">
       <c r="E200" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B201" s="7" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="201">
+      <c r="C201" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D201" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="E201" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+      <c r="F201" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="202">
       <c r="E202" s="7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="203">
       <c r="E203" s="7" t="s">
-        <v>307</v>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="E204" s="7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="E205" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E206" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="G206" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="E207" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G207" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -16266,13 +16603,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -16291,11 +16628,11 @@
         <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3">
@@ -16307,7 +16644,7 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4">
@@ -16316,31 +16653,31 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
       <c r="E5" s="7" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" s="7" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7">
@@ -16349,40 +16686,40 @@
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8">
       <c r="G8" s="7" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9">
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10">
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11">
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12">
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13">
@@ -16396,11 +16733,11 @@
         <v>16</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14">
@@ -16408,11 +16745,11 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15">
@@ -16426,11 +16763,11 @@
         <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16">
@@ -16438,11 +16775,11 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17">
@@ -16456,10 +16793,10 @@
         <v>64</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18">
@@ -16470,7 +16807,7 @@
         <v>48</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19">
@@ -16478,7 +16815,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>243</v>
@@ -16492,7 +16829,7 @@
         <v>57</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>243</v>
@@ -16503,10 +16840,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22">
@@ -16514,13 +16851,13 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23">
@@ -16528,10 +16865,10 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24">
@@ -16539,10 +16876,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25">
@@ -16550,10 +16887,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26">
@@ -16561,13 +16898,13 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27">
@@ -16575,10 +16912,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28">
@@ -16589,7 +16926,7 @@
         <v>48</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29">
@@ -16597,10 +16934,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30">
@@ -16610,7 +16947,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="I30" s="7" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="31">
@@ -16618,13 +16955,13 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="F31" s="7" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32">
@@ -16632,10 +16969,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33">
@@ -16643,10 +16980,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="G33" s="7" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34">
@@ -16654,16 +16991,16 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="F34" s="7" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35">
@@ -16671,10 +17008,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="H35" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36">
@@ -16683,7 +17020,7 @@
       <c r="D36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
     </row>
     <row r="37">
@@ -16691,10 +17028,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="H37" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38">
@@ -16704,7 +17041,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="I38" s="7" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="39">
@@ -16712,13 +17049,13 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="F39" s="7" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="40">
@@ -16726,10 +17063,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>243</v>
@@ -16740,7 +17077,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="G41" s="7" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="J41" s="7" t="s">
         <v>243</v>
@@ -16751,7 +17088,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="G42" s="7" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>243</v>
@@ -16762,13 +17099,13 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="G43" s="7" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44">
@@ -16777,7 +17114,7 @@
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="I44" s="7" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="45">
@@ -16786,7 +17123,7 @@
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="I45" s="7" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46">
@@ -16794,10 +17131,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47">
@@ -16805,10 +17142,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48">
@@ -16816,7 +17153,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="I48" s="7" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
     </row>
     <row r="49">
@@ -16824,7 +17161,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="I49" s="7" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="50">
@@ -16832,7 +17169,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="I50" s="7" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51">
@@ -16840,7 +17177,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="I51" s="7" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52">
@@ -16848,7 +17185,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="I52" s="7" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="J52" s="7" t="s">
         <v>243</v>
@@ -16865,7 +17202,7 @@
         <v>64</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54">
@@ -16893,10 +17230,10 @@
         <v>92</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56">
@@ -16907,7 +17244,7 @@
         <v>48</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="57">
@@ -16915,10 +17252,10 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58">
@@ -16932,10 +17269,10 @@
         <v>92</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="59">
@@ -16943,10 +17280,10 @@
       <c r="C59" s="22"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="60">
@@ -16960,10 +17297,10 @@
         <v>101</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="61">
@@ -16974,7 +17311,7 @@
         <v>48</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="62">
@@ -16982,10 +17319,10 @@
       <c r="C62" s="22"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="63">
@@ -16999,10 +17336,10 @@
         <v>101</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="64">
@@ -17010,10 +17347,10 @@
       <c r="C64" s="22"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65">
@@ -17044,7 +17381,7 @@
         <v>48</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="67">
@@ -17053,10 +17390,10 @@
       <c r="C67" s="22"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="68">
@@ -17065,10 +17402,10 @@
       <c r="C68" s="22"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
     </row>
     <row r="69">
@@ -17077,10 +17414,10 @@
       <c r="C69" s="22"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="70">
@@ -17089,10 +17426,10 @@
       <c r="C70" s="22"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71">
@@ -17101,13 +17438,13 @@
       <c r="C71" s="22"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="72">
@@ -17116,10 +17453,10 @@
       <c r="C72" s="22"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="73">
@@ -17128,10 +17465,10 @@
       <c r="C73" s="22"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74">
@@ -17140,13 +17477,13 @@
       <c r="C74" s="22"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="75">
@@ -17163,10 +17500,10 @@
         <v>116</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76">
@@ -17174,10 +17511,10 @@
       <c r="C76" s="22"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
     </row>
     <row r="77">
@@ -17188,10 +17525,10 @@
         <v>48</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
     </row>
     <row r="78">
@@ -17199,10 +17536,10 @@
       <c r="C78" s="22"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="79">
@@ -17210,10 +17547,10 @@
       <c r="C79" s="22"/>
       <c r="D79" s="7"/>
       <c r="I79" s="7" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
     </row>
     <row r="80">
@@ -17227,10 +17564,10 @@
         <v>116</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81">
@@ -17238,10 +17575,10 @@
       <c r="C81" s="22"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82">
@@ -17249,10 +17586,10 @@
       <c r="C82" s="22"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I82" s="22" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83">
@@ -17262,7 +17599,7 @@
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="I83" s="7" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="84">
@@ -17270,13 +17607,13 @@
       <c r="C84" s="22"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="85">
@@ -17284,10 +17621,10 @@
       <c r="C85" s="22"/>
       <c r="D85" s="7"/>
       <c r="F85" s="7" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="86">
@@ -17295,10 +17632,10 @@
       <c r="C86" s="22"/>
       <c r="D86" s="7"/>
       <c r="F86" s="7" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I86" s="7" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87">
@@ -17306,16 +17643,16 @@
       <c r="C87" s="22"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88">
@@ -17323,10 +17660,10 @@
       <c r="C88" s="22"/>
       <c r="D88" s="7"/>
       <c r="G88" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="89">
@@ -17335,7 +17672,7 @@
       <c r="D89" s="7"/>
       <c r="G89" s="7"/>
       <c r="I89" s="7" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
     </row>
     <row r="90">
@@ -17343,10 +17680,10 @@
       <c r="C90" s="22"/>
       <c r="D90" s="7"/>
       <c r="G90" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="I90" s="7" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="91">
@@ -17356,7 +17693,7 @@
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
       <c r="I91" s="7" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92">
@@ -17364,13 +17701,13 @@
       <c r="C92" s="22"/>
       <c r="D92" s="7"/>
       <c r="E92" s="7" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I92" s="7" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93">
@@ -17378,10 +17715,10 @@
       <c r="C93" s="22"/>
       <c r="D93" s="7"/>
       <c r="F93" s="7" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>243</v>
@@ -17392,7 +17729,7 @@
       <c r="C94" s="22"/>
       <c r="D94" s="7"/>
       <c r="F94" s="7" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>243</v>
@@ -17403,7 +17740,7 @@
       <c r="C95" s="22"/>
       <c r="D95" s="7"/>
       <c r="F95" s="7" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="J95" s="7" t="s">
         <v>243</v>
@@ -17414,13 +17751,13 @@
       <c r="C96" s="22"/>
       <c r="D96" s="7"/>
       <c r="F96" s="7" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="97">
@@ -17428,7 +17765,7 @@
       <c r="C97" s="22"/>
       <c r="D97" s="7"/>
       <c r="I97" s="7" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="98">
@@ -17436,7 +17773,7 @@
       <c r="C98" s="22"/>
       <c r="D98" s="7"/>
       <c r="I98" s="7" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
     <row r="99">
@@ -17444,10 +17781,10 @@
       <c r="C99" s="22"/>
       <c r="D99" s="7"/>
       <c r="E99" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I99" s="7" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="100">
@@ -17461,10 +17798,10 @@
         <v>125</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I100" s="7" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="101">
@@ -17472,10 +17809,10 @@
       <c r="C101" s="22"/>
       <c r="D101" s="7"/>
       <c r="E101" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="102">
@@ -17489,10 +17826,10 @@
         <v>125</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="103">
@@ -17500,10 +17837,10 @@
       <c r="C103" s="22"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104">
@@ -17534,10 +17871,10 @@
         <v>134</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="106">
@@ -17545,10 +17882,10 @@
       <c r="C106" s="22"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107">
@@ -17556,10 +17893,10 @@
       <c r="C107" s="22"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
     </row>
     <row r="108">
@@ -17567,10 +17904,10 @@
       <c r="C108" s="22"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109">
@@ -17581,10 +17918,10 @@
         <v>108</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110">
@@ -17592,13 +17929,13 @@
       <c r="C110" s="22"/>
       <c r="D110" s="7"/>
       <c r="E110" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I110" s="7" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
     </row>
     <row r="111">
@@ -17606,10 +17943,10 @@
       <c r="C111" s="22"/>
       <c r="D111" s="7"/>
       <c r="E111" s="7" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
     </row>
     <row r="112">
@@ -17617,10 +17954,10 @@
       <c r="C112" s="22"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="113">
@@ -17634,10 +17971,10 @@
         <v>134</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="114">
@@ -17645,10 +17982,10 @@
       <c r="C114" s="22"/>
       <c r="D114" s="7"/>
       <c r="E114" s="7" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
     </row>
     <row r="115">
@@ -17656,10 +17993,10 @@
       <c r="C115" s="22"/>
       <c r="D115" s="7"/>
       <c r="E115" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116">
@@ -17673,10 +18010,10 @@
         <v>143</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117">
@@ -17684,10 +18021,10 @@
       <c r="C117" s="22"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="118">
@@ -17695,10 +18032,10 @@
       <c r="C118" s="22"/>
       <c r="D118" s="7"/>
       <c r="E118" s="7" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="I118" s="7" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
     </row>
     <row r="119">
@@ -17706,10 +18043,10 @@
       <c r="C119" s="22"/>
       <c r="D119" s="7"/>
       <c r="E119" s="7" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="I119" s="7" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120">
@@ -17720,10 +18057,10 @@
         <v>108</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="I120" s="7" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="121">
@@ -17731,10 +18068,10 @@
       <c r="C121" s="22"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
     </row>
     <row r="122">
@@ -17742,10 +18079,10 @@
       <c r="C122" s="22"/>
       <c r="D122" s="7"/>
       <c r="E122" s="7" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="I122" s="7" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
     </row>
     <row r="123">
@@ -17753,10 +18090,10 @@
       <c r="C123" s="22"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="I123" s="7" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="124">
@@ -17787,10 +18124,10 @@
         <v>149</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="I125" s="7" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126">
@@ -17801,10 +18138,10 @@
         <v>28</v>
       </c>
       <c r="I126" s="7" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="127">
@@ -17812,13 +18149,13 @@
       <c r="C127" s="22"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="I127" s="7" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="J127" s="7" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="128">
@@ -17826,10 +18163,10 @@
       <c r="C128" s="22"/>
       <c r="D128" s="7"/>
       <c r="E128" s="7" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="I128" s="7" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="J128" s="7" t="s">
         <v>243</v>
@@ -17840,16 +18177,16 @@
       <c r="C129" s="22"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="G129" s="7" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="I129" s="7" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
     <row r="130">
@@ -17858,10 +18195,10 @@
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
       <c r="G130" s="7" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131">
@@ -17870,10 +18207,10 @@
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
       <c r="G131" s="7" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="I131" s="7" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="132">
@@ -17882,13 +18219,13 @@
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
       <c r="G132" s="7" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="I132" s="7" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="J132" s="7" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
     </row>
     <row r="133">
@@ -17897,10 +18234,10 @@
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
       <c r="G133" s="7" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="I133" s="7" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
     </row>
     <row r="134">
@@ -17909,10 +18246,10 @@
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
       <c r="G134" s="7" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="I134" s="7" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
     </row>
     <row r="135">
@@ -17921,10 +18258,10 @@
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
       <c r="G135" s="7" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="I135" s="7" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
     </row>
     <row r="136">
@@ -17933,10 +18270,10 @@
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
       <c r="G136" s="7" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="I136" s="7" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
     </row>
     <row r="137">
@@ -17945,7 +18282,7 @@
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
       <c r="G137" s="7" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="J137" s="7" t="s">
         <v>243</v>
@@ -17957,7 +18294,7 @@
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
       <c r="G138" s="7" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="J138" s="7" t="s">
         <v>243</v>
@@ -17969,7 +18306,7 @@
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
       <c r="I139" s="7" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
     </row>
     <row r="140">
@@ -17978,7 +18315,7 @@
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
       <c r="I140" s="7" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
     </row>
     <row r="141">
@@ -17987,7 +18324,7 @@
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
       <c r="I141" s="7" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
     </row>
     <row r="142">
@@ -17996,7 +18333,7 @@
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
       <c r="I142" s="7" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="143">
@@ -18015,44 +18352,44 @@
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="B144" s="7">
         <v>400.0</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="I144" s="7" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" s="7"/>
       <c r="E145" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="F145" s="7" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="I145" s="7" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" s="7"/>
       <c r="E146" s="7"/>
       <c r="I146" s="7" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" s="7"/>
       <c r="E147" s="7" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
     </row>
     <row r="148">
@@ -18060,19 +18397,19 @@
         <v>404.0</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="I148" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" s="7"/>
       <c r="E149" s="7" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="I149" s="7" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
     </row>
     <row r="150">
@@ -18080,18 +18417,18 @@
         <v>405.0</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="I150" s="7" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
     </row>
     <row r="151">
       <c r="E151" s="7" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="I151" s="7" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -18115,19 +18452,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2">
@@ -18135,10 +18472,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -18147,7 +18484,7 @@
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="6" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -18156,7 +18493,7 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="6" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -18165,7 +18502,7 @@
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="6" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -18174,20 +18511,20 @@
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -18196,7 +18533,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="6" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -18205,7 +18542,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="6" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -18214,7 +18551,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="6" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -18223,7 +18560,7 @@
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="6" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -18233,10 +18570,10 @@
         <v>80</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -18245,7 +18582,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -18254,7 +18591,7 @@
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="6" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -18263,7 +18600,7 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="6" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -18272,7 +18609,7 @@
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="6" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -18282,10 +18619,10 @@
         <v>77</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -18294,7 +18631,7 @@
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="6" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -18303,7 +18640,7 @@
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="6" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -18312,7 +18649,7 @@
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="6" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -18321,7 +18658,7 @@
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -18361,14 +18698,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="B17:B21"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>